<commit_message>
updated branch with edited data set for machine learning ending in ML and tableau ending in rev
</commit_message>
<xml_diff>
--- a/DataSets/LCDataDictionary.xlsx
+++ b/DataSets/LCDataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Data Analytics and I\Project 3 Potential\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carladams/Documents/DVAB/BLPFinalProject/DataSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F813B7F-4C60-46F9-A4CE-22A516ECB106}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93AD9F7-3284-DB4D-B6EB-FB608602BD6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28860" yWindow="460" windowWidth="29040" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1203,7 +1203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1385,7 +1385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1568,6 +1568,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1819,7 +1825,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1857,6 +1863,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2258,19 +2266,19 @@
   <dimension ref="A1:K154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A145" sqref="A145:B145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="16" t="s">
         <v>99</v>
       </c>
@@ -2278,7 +2286,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="4" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>291</v>
       </c>
@@ -2287,7 +2295,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="4" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>295</v>
       </c>
@@ -2296,7 +2304,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -2305,7 +2313,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="5" customFormat="1">
       <c r="A5" s="9" t="s">
         <v>285</v>
       </c>
@@ -2314,7 +2322,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="16">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2323,7 +2331,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="4" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
@@ -2332,7 +2340,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="4" customFormat="1">
       <c r="A8" s="7" t="s">
         <v>252</v>
       </c>
@@ -2341,7 +2349,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>114</v>
       </c>
@@ -2350,7 +2358,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="4" customFormat="1">
       <c r="A10" s="9" t="s">
         <v>296</v>
       </c>
@@ -2359,7 +2367,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>297</v>
       </c>
@@ -2368,7 +2376,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="4" customFormat="1">
       <c r="A12" s="9" t="s">
         <v>105</v>
       </c>
@@ -2377,7 +2385,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="16">
       <c r="A13" s="7" t="s">
         <v>226</v>
       </c>
@@ -2386,7 +2394,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="16">
       <c r="A14" s="3" t="s">
         <v>106</v>
       </c>
@@ -2395,7 +2403,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="16">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -2404,7 +2412,7 @@
       </c>
       <c r="C15" s="24"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="4" customFormat="1">
       <c r="A16" s="9" t="s">
         <v>298</v>
       </c>
@@ -2413,7 +2421,7 @@
       </c>
       <c r="C16" s="24"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -2422,7 +2430,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -2431,7 +2439,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="4" customFormat="1">
       <c r="A19" s="7" t="s">
         <v>255</v>
       </c>
@@ -2440,7 +2448,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -2449,7 +2457,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2458,7 +2466,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A22" s="3" t="s">
         <v>166</v>
       </c>
@@ -2467,7 +2475,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2476,7 +2484,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2485,7 +2493,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2494,7 +2502,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -2503,7 +2511,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -2512,7 +2520,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -2521,7 +2529,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="4" customFormat="1" ht="16">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2530,7 +2538,7 @@
       </c>
       <c r="C29" s="24"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="4" customFormat="1">
       <c r="A30" s="9" t="s">
         <v>277</v>
       </c>
@@ -2539,7 +2547,7 @@
       </c>
       <c r="C30" s="24"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2548,7 +2556,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="4" customFormat="1">
       <c r="A32" s="9" t="s">
         <v>287</v>
       </c>
@@ -2557,7 +2565,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="4" customFormat="1">
       <c r="A33" s="9" t="s">
         <v>289</v>
       </c>
@@ -2566,7 +2574,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="16">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -2575,7 +2583,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="16">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2584,7 +2592,7 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="16">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2593,7 +2601,7 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="16">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -2604,7 +2612,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="16">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2613,7 +2621,7 @@
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="16">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2622,7 +2630,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="16">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2631,7 +2639,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="16" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -2640,7 +2648,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="16">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -2649,7 +2657,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="16" customHeight="1">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2658,7 +2666,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="16">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -2667,7 +2675,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="9" t="s">
         <v>283</v>
       </c>
@@ -2676,7 +2684,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="16">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2688,7 +2696,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" s="9" t="s">
         <v>299</v>
       </c>
@@ -2700,7 +2708,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="9" t="s">
         <v>124</v>
       </c>
@@ -2712,7 +2720,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="9" t="s">
         <v>125</v>
       </c>
@@ -2721,7 +2729,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="9" t="s">
         <v>111</v>
       </c>
@@ -2730,7 +2738,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="9" t="s">
         <v>300</v>
       </c>
@@ -2739,7 +2747,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="16">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2748,7 +2756,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="8" t="s">
         <v>108</v>
       </c>
@@ -2757,7 +2765,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="16">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2766,7 +2774,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="9" t="s">
         <v>273</v>
       </c>
@@ -2775,7 +2783,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="9" t="s">
         <v>301</v>
       </c>
@@ -2784,7 +2792,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="8" t="s">
         <v>302</v>
       </c>
@@ -2793,7 +2801,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="9" t="s">
         <v>304</v>
       </c>
@@ -2802,7 +2810,7 @@
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="9" t="s">
         <v>305</v>
       </c>
@@ -2811,7 +2819,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" s="6" customFormat="1" ht="16">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -2820,7 +2828,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="9" t="s">
         <v>104</v>
       </c>
@@ -2829,7 +2837,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="9" t="s">
         <v>116</v>
       </c>
@@ -2837,7 +2845,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="9" t="s">
         <v>123</v>
       </c>
@@ -2845,7 +2853,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="9" t="s">
         <v>117</v>
       </c>
@@ -2853,7 +2861,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="9" t="s">
         <v>115</v>
       </c>
@@ -2861,7 +2869,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="9" t="s">
         <v>122</v>
       </c>
@@ -2869,7 +2877,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="9" t="s">
         <v>127</v>
       </c>
@@ -2877,7 +2885,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
@@ -2885,7 +2893,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="9" t="s">
         <v>126</v>
       </c>
@@ -2893,7 +2901,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="9" t="s">
         <v>109</v>
       </c>
@@ -2901,7 +2909,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="9" t="s">
         <v>121</v>
       </c>
@@ -2909,7 +2917,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="9" t="s">
         <v>120</v>
       </c>
@@ -2917,7 +2925,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="9" t="s">
         <v>119</v>
       </c>
@@ -2927,7 +2935,7 @@
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="9" t="s">
         <v>110</v>
       </c>
@@ -2935,7 +2943,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="16">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
@@ -2943,7 +2951,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="9" t="s">
         <v>266</v>
       </c>
@@ -2951,7 +2959,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="9" t="s">
         <v>269</v>
       </c>
@@ -2959,7 +2967,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="9" t="s">
         <v>271</v>
       </c>
@@ -2967,7 +2975,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="9" t="s">
         <v>335</v>
       </c>
@@ -2975,7 +2983,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="9" t="s">
         <v>279</v>
       </c>
@@ -2983,7 +2991,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" s="9" t="s">
         <v>281</v>
       </c>
@@ -2991,7 +2999,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="16">
       <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
@@ -2999,7 +3007,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="16">
       <c r="A83" s="3" t="s">
         <v>36</v>
       </c>
@@ -3007,7 +3015,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="9" t="s">
         <v>118</v>
       </c>
@@ -3015,7 +3023,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="9" t="s">
         <v>306</v>
       </c>
@@ -3023,7 +3031,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="32">
       <c r="A86" s="3" t="s">
         <v>129</v>
       </c>
@@ -3031,7 +3039,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="16">
       <c r="A87" s="3" t="s">
         <v>30</v>
       </c>
@@ -3039,7 +3047,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" s="9" t="s">
         <v>103</v>
       </c>
@@ -3047,7 +3055,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="16">
       <c r="A89" s="3" t="s">
         <v>18</v>
       </c>
@@ -3055,7 +3063,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="16">
       <c r="A90" s="3" t="s">
         <v>15</v>
       </c>
@@ -3063,7 +3071,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="16">
       <c r="A91" s="7" t="s">
         <v>225</v>
       </c>
@@ -3071,7 +3079,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="16">
       <c r="A92" s="3" t="s">
         <v>31</v>
       </c>
@@ -3079,7 +3087,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="16">
       <c r="A93" s="3" t="s">
         <v>32</v>
       </c>
@@ -3087,7 +3095,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="16">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -3095,7 +3103,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" s="9" t="s">
         <v>107</v>
       </c>
@@ -3103,7 +3111,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="16">
       <c r="A96" s="3" t="s">
         <v>5</v>
       </c>
@@ -3111,7 +3119,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="16">
       <c r="A97" s="3" t="s">
         <v>19</v>
       </c>
@@ -3119,7 +3127,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="9" t="s">
         <v>128</v>
       </c>
@@ -3127,7 +3135,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" s="9" t="s">
         <v>113</v>
       </c>
@@ -3135,7 +3143,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" s="9" t="s">
         <v>112</v>
       </c>
@@ -3143,7 +3151,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="16">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -3151,7 +3159,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" s="9" t="s">
         <v>307</v>
       </c>
@@ -3159,7 +3167,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103" s="9" t="s">
         <v>275</v>
       </c>
@@ -3167,7 +3175,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2">
       <c r="A104" s="9" t="s">
         <v>308</v>
       </c>
@@ -3175,7 +3183,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2">
       <c r="A105" s="9" t="s">
         <v>293</v>
       </c>
@@ -3183,7 +3191,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2">
       <c r="A106" s="9" t="s">
         <v>100</v>
       </c>
@@ -3191,7 +3199,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="16">
       <c r="A107" s="3" t="s">
         <v>37</v>
       </c>
@@ -3199,7 +3207,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="16">
       <c r="A108" s="3" t="s">
         <v>38</v>
       </c>
@@ -3207,7 +3215,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="16">
       <c r="A109" s="3" t="s">
         <v>40</v>
       </c>
@@ -3215,7 +3223,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="16">
       <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
@@ -3223,7 +3231,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="16">
       <c r="A111" s="3" t="s">
         <v>39</v>
       </c>
@@ -3231,7 +3239,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2">
       <c r="A112" s="9" t="s">
         <v>217</v>
       </c>
@@ -3239,7 +3247,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="16">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -3247,7 +3255,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="16">
       <c r="A114" s="7" t="s">
         <v>294</v>
       </c>
@@ -3255,7 +3263,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2">
       <c r="A115" s="7" t="s">
         <v>257</v>
       </c>
@@ -3263,7 +3271,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2">
       <c r="A116" s="18" t="s">
         <v>247</v>
       </c>
@@ -3271,7 +3279,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2">
       <c r="A117" s="18" t="s">
         <v>310</v>
       </c>
@@ -3279,7 +3287,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2">
       <c r="A118" s="18" t="s">
         <v>312</v>
       </c>
@@ -3287,7 +3295,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2">
       <c r="A119" s="18" t="s">
         <v>314</v>
       </c>
@@ -3295,7 +3303,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2">
       <c r="A120" s="18" t="s">
         <v>316</v>
       </c>
@@ -3303,7 +3311,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2">
       <c r="A121" s="18" t="s">
         <v>318</v>
       </c>
@@ -3311,7 +3319,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2">
       <c r="A122" s="18" t="s">
         <v>320</v>
       </c>
@@ -3319,7 +3327,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2">
       <c r="A123" s="18" t="s">
         <v>322</v>
       </c>
@@ -3327,7 +3335,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2">
       <c r="A124" s="18" t="s">
         <v>324</v>
       </c>
@@ -3335,7 +3343,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2">
       <c r="A125" s="18" t="s">
         <v>336</v>
       </c>
@@ -3343,7 +3351,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2">
       <c r="A126" s="18" t="s">
         <v>327</v>
       </c>
@@ -3351,7 +3359,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2">
       <c r="A127" s="18" t="s">
         <v>329</v>
       </c>
@@ -3359,7 +3367,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2">
       <c r="A128" s="18" t="s">
         <v>331</v>
       </c>
@@ -3367,7 +3375,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2">
       <c r="A129" s="18" t="s">
         <v>333</v>
       </c>
@@ -3375,7 +3383,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2">
       <c r="A130" s="9" t="s">
         <v>347</v>
       </c>
@@ -3383,7 +3391,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2">
       <c r="A131" s="9" t="s">
         <v>348</v>
       </c>
@@ -3391,7 +3399,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2">
       <c r="A132" s="9" t="s">
         <v>349</v>
       </c>
@@ -3399,7 +3407,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2">
       <c r="A133" s="9" t="s">
         <v>350</v>
       </c>
@@ -3407,7 +3415,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2">
       <c r="A134" s="9" t="s">
         <v>351</v>
       </c>
@@ -3415,7 +3423,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2">
       <c r="A135" s="9" t="s">
         <v>352</v>
       </c>
@@ -3423,7 +3431,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2">
       <c r="A136" s="9" t="s">
         <v>353</v>
       </c>
@@ -3431,7 +3439,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2">
       <c r="A137" s="9" t="s">
         <v>354</v>
       </c>
@@ -3439,7 +3447,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2">
       <c r="A138" s="9" t="s">
         <v>355</v>
       </c>
@@ -3447,7 +3455,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2">
       <c r="A139" s="9" t="s">
         <v>356</v>
       </c>
@@ -3455,7 +3463,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2">
       <c r="A140" s="9" t="s">
         <v>357</v>
       </c>
@@ -3463,7 +3471,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2">
       <c r="A141" s="9" t="s">
         <v>358</v>
       </c>
@@ -3471,7 +3479,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2">
       <c r="A142" s="9" t="s">
         <v>359</v>
       </c>
@@ -3479,7 +3487,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2">
       <c r="A143" s="9" t="s">
         <v>360</v>
       </c>
@@ -3487,7 +3495,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2">
       <c r="A144" s="9" t="s">
         <v>361</v>
       </c>
@@ -3495,7 +3503,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2">
       <c r="A145" s="9" t="s">
         <v>362</v>
       </c>
@@ -3503,7 +3511,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2">
       <c r="A146" s="9" t="s">
         <v>345</v>
       </c>
@@ -3511,7 +3519,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2">
       <c r="A147" s="9" t="s">
         <v>346</v>
       </c>
@@ -3519,7 +3527,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2">
       <c r="A148" s="9" t="s">
         <v>363</v>
       </c>
@@ -3527,7 +3535,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2">
       <c r="A149" s="9" t="s">
         <v>340</v>
       </c>
@@ -3535,7 +3543,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2">
       <c r="A150" s="9" t="s">
         <v>364</v>
       </c>
@@ -3543,7 +3551,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2">
       <c r="A151" s="9" t="s">
         <v>365</v>
       </c>
@@ -3551,7 +3559,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2">
       <c r="A152" s="9" t="s">
         <v>366</v>
       </c>
@@ -3559,7 +3567,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="16">
       <c r="B154" s="13" t="s">
         <v>168</v>
       </c>
@@ -3578,19 +3586,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="235.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="235.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="235.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="235.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="15" t="s">
         <v>219</v>
       </c>
@@ -3598,7 +3606,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="9" t="s">
         <v>183</v>
       </c>
@@ -3609,8 +3617,8 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="25" t="s">
         <v>191</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -3620,8 +3628,8 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="25" t="s">
         <v>192</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -3631,7 +3639,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="9" t="s">
         <v>190</v>
       </c>
@@ -3642,15 +3650,15 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:6" s="6" customFormat="1">
+      <c r="A6" s="25" t="s">
         <v>285</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
@@ -3660,8 +3668,8 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:6" s="6" customFormat="1">
+      <c r="A8" s="25" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -3669,8 +3677,8 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="26" t="s">
         <v>252</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -3679,8 +3687,8 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="25" t="s">
         <v>114</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -3690,7 +3698,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="9" t="s">
         <v>193</v>
       </c>
@@ -3701,8 +3709,8 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="25" t="s">
         <v>195</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -3711,8 +3719,8 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="25" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -3721,8 +3729,8 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="25" t="s">
         <v>106</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -3732,8 +3740,8 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="8" t="s">
         <v>187</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -3743,8 +3751,8 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="25" t="s">
         <v>196</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -3754,8 +3762,8 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="25" t="s">
         <v>197</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -3765,7 +3773,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
@@ -3776,8 +3784,8 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:6" s="6" customFormat="1">
+      <c r="A19" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -3785,7 +3793,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="7" t="s">
         <v>255</v>
       </c>
@@ -3796,7 +3804,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="9" t="s">
         <v>198</v>
       </c>
@@ -3806,8 +3814,8 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:6">
+      <c r="A22" s="7" t="s">
         <v>239</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -3817,8 +3825,8 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:6">
+      <c r="A23" s="8" t="s">
         <v>166</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -3828,8 +3836,8 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" s="25" t="s">
         <v>177</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -3839,7 +3847,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="9" t="s">
         <v>185</v>
       </c>
@@ -3850,7 +3858,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="9" t="s">
         <v>173</v>
       </c>
@@ -3861,7 +3869,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="9" t="s">
         <v>200</v>
       </c>
@@ -3872,7 +3880,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="9" t="s">
         <v>199</v>
       </c>
@@ -3883,8 +3891,8 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="25" t="s">
         <v>171</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -3894,7 +3902,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="9" t="s">
         <v>8</v>
       </c>
@@ -3905,7 +3913,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="9" t="s">
         <v>179</v>
       </c>
@@ -3916,7 +3924,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
@@ -3926,8 +3934,8 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="25" t="s">
         <v>277</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -3936,7 +3944,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="9" t="s">
         <v>161</v>
       </c>
@@ -3947,7 +3955,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="9" t="s">
         <v>216</v>
       </c>
@@ -3958,8 +3966,8 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="25" t="s">
         <v>287</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -3969,8 +3977,8 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" s="25" t="s">
         <v>289</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -3980,8 +3988,8 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+    <row r="38" spans="1:6">
+      <c r="A38" s="25" t="s">
         <v>201</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -3991,8 +3999,8 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+    <row r="39" spans="1:6">
+      <c r="A39" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -4002,8 +4010,8 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+    <row r="40" spans="1:6">
+      <c r="A40" s="25" t="s">
         <v>172</v>
       </c>
       <c r="B40" s="9" t="s">
@@ -4013,8 +4021,8 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+    <row r="41" spans="1:6" ht="16">
+      <c r="A41" s="25" t="s">
         <v>182</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -4023,7 +4031,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="9" t="s">
         <v>186</v>
       </c>
@@ -4033,8 +4041,8 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43" s="25" t="s">
         <v>170</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -4043,8 +4051,8 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" s="25" t="s">
         <v>283</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -4053,7 +4061,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="9" t="s">
         <v>169</v>
       </c>
@@ -4063,8 +4071,8 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+    <row r="46" spans="1:6">
+      <c r="A46" s="25" t="s">
         <v>124</v>
       </c>
       <c r="B46" s="9" t="s">
@@ -4074,8 +4082,8 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:6">
+      <c r="A47" s="25" t="s">
         <v>125</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -4084,8 +4092,8 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48" s="25" t="s">
         <v>111</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -4094,8 +4102,8 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" s="25" t="s">
         <v>208</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -4104,7 +4112,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="9" t="s">
         <v>160</v>
       </c>
@@ -4114,8 +4122,8 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51" s="25" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="9" t="s">
@@ -4124,8 +4132,8 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+    <row r="52" spans="1:6">
+      <c r="A52" s="25" t="s">
         <v>101</v>
       </c>
       <c r="B52" s="9" t="s">
@@ -4134,8 +4142,8 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+    <row r="53" spans="1:6">
+      <c r="A53" s="25" t="s">
         <v>273</v>
       </c>
       <c r="B53" s="9" t="s">
@@ -4143,8 +4151,8 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="54" spans="1:6">
+      <c r="A54" s="25" t="s">
         <v>202</v>
       </c>
       <c r="B54" s="9" t="s">
@@ -4152,8 +4160,8 @@
       </c>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" s="25" t="s">
         <v>203</v>
       </c>
       <c r="B55" s="9" t="s">
@@ -4161,8 +4169,8 @@
       </c>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+    <row r="56" spans="1:6">
+      <c r="A56" s="25" t="s">
         <v>204</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -4170,8 +4178,8 @@
       </c>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+    <row r="57" spans="1:6">
+      <c r="A57" s="25" t="s">
         <v>207</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -4179,8 +4187,8 @@
       </c>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+    <row r="58" spans="1:6">
+      <c r="A58" s="25" t="s">
         <v>205</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -4188,8 +4196,8 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="59" spans="1:6">
+      <c r="A59" s="25" t="s">
         <v>206</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -4197,8 +4205,8 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="60" spans="1:6">
+      <c r="A60" s="25" t="s">
         <v>104</v>
       </c>
       <c r="B60" s="9" t="s">
@@ -4206,8 +4214,8 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="1:6">
+      <c r="A61" s="25" t="s">
         <v>116</v>
       </c>
       <c r="B61" s="9" t="s">
@@ -4215,8 +4223,8 @@
       </c>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+    <row r="62" spans="1:6">
+      <c r="A62" s="25" t="s">
         <v>123</v>
       </c>
       <c r="B62" s="9" t="s">
@@ -4224,8 +4232,8 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+    <row r="63" spans="1:6">
+      <c r="A63" s="25" t="s">
         <v>117</v>
       </c>
       <c r="B63" s="9" t="s">
@@ -4233,8 +4241,8 @@
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+    <row r="64" spans="1:6">
+      <c r="A64" s="25" t="s">
         <v>115</v>
       </c>
       <c r="B64" s="9" t="s">
@@ -4242,8 +4250,8 @@
       </c>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+    <row r="65" spans="1:6">
+      <c r="A65" s="25" t="s">
         <v>122</v>
       </c>
       <c r="B65" s="9" t="s">
@@ -4251,8 +4259,8 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+    <row r="66" spans="1:6">
+      <c r="A66" s="25" t="s">
         <v>127</v>
       </c>
       <c r="B66" s="9" t="s">
@@ -4260,8 +4268,8 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+    <row r="67" spans="1:6">
+      <c r="A67" s="25" t="s">
         <v>102</v>
       </c>
       <c r="B67" s="9" t="s">
@@ -4269,8 +4277,8 @@
       </c>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+    <row r="68" spans="1:6">
+      <c r="A68" s="25" t="s">
         <v>126</v>
       </c>
       <c r="B68" s="9" t="s">
@@ -4278,8 +4286,8 @@
       </c>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+    <row r="69" spans="1:6">
+      <c r="A69" s="25" t="s">
         <v>109</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -4287,8 +4295,8 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+    <row r="70" spans="1:6">
+      <c r="A70" s="25" t="s">
         <v>121</v>
       </c>
       <c r="B70" s="9" t="s">
@@ -4297,8 +4305,8 @@
       <c r="D70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+    <row r="71" spans="1:6">
+      <c r="A71" s="25" t="s">
         <v>120</v>
       </c>
       <c r="B71" s="9" t="s">
@@ -4306,8 +4314,8 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+    <row r="72" spans="1:6">
+      <c r="A72" s="25" t="s">
         <v>119</v>
       </c>
       <c r="B72" s="9" t="s">
@@ -4315,8 +4323,8 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+    <row r="73" spans="1:6">
+      <c r="A73" s="25" t="s">
         <v>110</v>
       </c>
       <c r="B73" s="9" t="s">
@@ -4325,8 +4333,8 @@
       <c r="D73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
+    <row r="74" spans="1:6">
+      <c r="A74" s="25" t="s">
         <v>266</v>
       </c>
       <c r="B74" s="8" t="s">
@@ -4335,8 +4343,8 @@
       <c r="D74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+    <row r="75" spans="1:6">
+      <c r="A75" s="25" t="s">
         <v>269</v>
       </c>
       <c r="B75" s="9" t="s">
@@ -4345,8 +4353,8 @@
       <c r="D75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
+    <row r="76" spans="1:6">
+      <c r="A76" s="25" t="s">
         <v>271</v>
       </c>
       <c r="B76" s="9" t="s">
@@ -4354,8 +4362,8 @@
       </c>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
+    <row r="77" spans="1:6">
+      <c r="A77" s="25" t="s">
         <v>335</v>
       </c>
       <c r="B77" s="9" t="s">
@@ -4363,8 +4371,8 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
+    <row r="78" spans="1:6">
+      <c r="A78" s="25" t="s">
         <v>279</v>
       </c>
       <c r="B78" s="9" t="s">
@@ -4373,8 +4381,8 @@
       <c r="D78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
+    <row r="79" spans="1:6">
+      <c r="A79" s="25" t="s">
         <v>281</v>
       </c>
       <c r="B79" s="9" t="s">
@@ -4383,8 +4391,8 @@
       <c r="D79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+    <row r="80" spans="1:6">
+      <c r="A80" s="25" t="s">
         <v>209</v>
       </c>
       <c r="B80" s="9" t="s">
@@ -4392,8 +4400,8 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+    <row r="81" spans="1:6">
+      <c r="A81" s="25" t="s">
         <v>118</v>
       </c>
       <c r="B81" s="9" t="s">
@@ -4402,8 +4410,8 @@
       <c r="D81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+    <row r="82" spans="1:6">
+      <c r="A82" s="25" t="s">
         <v>194</v>
       </c>
       <c r="B82" s="9" t="s">
@@ -4412,8 +4420,8 @@
       <c r="D82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
+    <row r="83" spans="1:6">
+      <c r="A83" s="25" t="s">
         <v>103</v>
       </c>
       <c r="B83" s="9" t="s">
@@ -4421,8 +4429,8 @@
       </c>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
+    <row r="84" spans="1:6">
+      <c r="A84" s="25" t="s">
         <v>210</v>
       </c>
       <c r="B84" s="9" t="s">
@@ -4430,8 +4438,8 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
+    <row r="85" spans="1:6">
+      <c r="A85" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B85" s="9" t="s">
@@ -4439,7 +4447,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="9" t="s">
         <v>189</v>
       </c>
@@ -4448,7 +4456,7 @@
       </c>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="9" t="s">
         <v>188</v>
       </c>
@@ -4457,8 +4465,8 @@
       </c>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+    <row r="88" spans="1:6">
+      <c r="A88" s="25" t="s">
         <v>212</v>
       </c>
       <c r="B88" s="9" t="s">
@@ -4466,8 +4474,8 @@
       </c>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+    <row r="89" spans="1:6">
+      <c r="A89" s="25" t="s">
         <v>213</v>
       </c>
       <c r="B89" s="9" t="s">
@@ -4475,7 +4483,7 @@
       </c>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="9" t="s">
         <v>174</v>
       </c>
@@ -4484,7 +4492,7 @@
       </c>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="9" t="s">
         <v>176</v>
       </c>
@@ -4494,8 +4502,8 @@
       <c r="D91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
+    <row r="92" spans="1:6" s="6" customFormat="1">
+      <c r="A92" s="25" t="s">
         <v>107</v>
       </c>
       <c r="B92" s="9" t="s">
@@ -4503,8 +4511,8 @@
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+    <row r="93" spans="1:6">
+      <c r="A93" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B93" s="9" t="s">
@@ -4513,7 +4521,7 @@
       <c r="D93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="9" t="s">
         <v>19</v>
       </c>
@@ -4521,87 +4529,87 @@
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+    <row r="95" spans="1:6">
+      <c r="A95" s="25" t="s">
         <v>128</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="9" t="s">
+    <row r="96" spans="1:6">
+      <c r="A96" s="25" t="s">
         <v>113</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" s="25" t="s">
         <v>112</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" s="25" t="s">
         <v>275</v>
       </c>
       <c r="B98" s="9" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="9" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" s="25" t="s">
         <v>293</v>
       </c>
       <c r="B99" s="9" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
+    <row r="100" spans="1:2">
+      <c r="A100" s="25" t="s">
         <v>100</v>
       </c>
       <c r="B100" s="9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
+    <row r="101" spans="1:2">
+      <c r="A101" s="25" t="s">
         <v>217</v>
       </c>
       <c r="B101" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
+    <row r="102" spans="1:2">
+      <c r="A102" s="25" t="s">
         <v>215</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
+    <row r="103" spans="1:2">
+      <c r="A103" s="25" t="s">
         <v>211</v>
       </c>
       <c r="B103" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="9" t="s">
+    <row r="104" spans="1:2">
+      <c r="A104" s="25" t="s">
         <v>214</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2">
       <c r="A105" s="9" t="s">
         <v>16</v>
       </c>
@@ -4609,7 +4617,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2">
       <c r="A106" s="7" t="s">
         <v>257</v>
       </c>
@@ -4617,7 +4625,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2">
       <c r="A107" s="22" t="s">
         <v>247</v>
       </c>
@@ -4625,7 +4633,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2">
       <c r="A108" s="18" t="s">
         <v>310</v>
       </c>
@@ -4633,7 +4641,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2">
       <c r="A109" s="18" t="s">
         <v>312</v>
       </c>
@@ -4641,7 +4649,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2">
       <c r="A110" s="18" t="s">
         <v>314</v>
       </c>
@@ -4649,7 +4657,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2">
       <c r="A111" s="18" t="s">
         <v>316</v>
       </c>
@@ -4657,7 +4665,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2">
       <c r="A112" s="18" t="s">
         <v>318</v>
       </c>
@@ -4665,7 +4673,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2">
       <c r="A113" s="18" t="s">
         <v>320</v>
       </c>
@@ -4673,7 +4681,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2">
       <c r="A114" s="18" t="s">
         <v>322</v>
       </c>
@@ -4681,7 +4689,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2">
       <c r="A115" s="18" t="s">
         <v>324</v>
       </c>
@@ -4689,7 +4697,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2">
       <c r="A116" s="18" t="s">
         <v>336</v>
       </c>
@@ -4697,7 +4705,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2">
       <c r="A117" s="18" t="s">
         <v>327</v>
       </c>
@@ -4705,7 +4713,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2">
       <c r="A118" s="18" t="s">
         <v>329</v>
       </c>
@@ -4713,7 +4721,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2">
       <c r="A119" s="18" t="s">
         <v>331</v>
       </c>
@@ -4721,7 +4729,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2">
       <c r="A120" s="18" t="s">
         <v>333</v>
       </c>
@@ -4729,7 +4737,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2">
       <c r="A121" s="9" t="s">
         <v>362</v>
       </c>
@@ -4737,7 +4745,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="16">
       <c r="B123" s="13" t="s">
         <v>168</v>
       </c>
@@ -4760,17 +4768,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="17" t="s">
         <v>227</v>
       </c>
@@ -4778,7 +4786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="18" t="s">
         <v>228</v>
       </c>
@@ -4786,7 +4794,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="18" t="s">
         <v>229</v>
       </c>
@@ -4794,7 +4802,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16">
       <c r="A4" s="18" t="s">
         <v>230</v>
       </c>
@@ -4802,7 +4810,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="18" t="s">
         <v>243</v>
       </c>
@@ -4810,7 +4818,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16">
       <c r="A6" s="18" t="s">
         <v>231</v>
       </c>
@@ -4818,7 +4826,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="18" t="s">
         <v>245</v>
       </c>
@@ -4826,7 +4834,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="18" t="s">
         <v>232</v>
       </c>
@@ -4834,7 +4842,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="18" t="s">
         <v>233</v>
       </c>
@@ -4842,7 +4850,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="32">
       <c r="A10" s="18" t="s">
         <v>234</v>
       </c>
@@ -4850,11 +4858,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>

</xml_diff>